<commit_message>
Updated my 450 DSA, Did some Array Question
</commit_message>
<xml_diff>
--- a/Codes/FINAL450.xlsx
+++ b/Codes/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\Git\Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499E666-4505-425A-AD6C-167049059B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1420,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1857,18 +1854,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1888,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21">
@@ -1935,7 +1932,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -2012,7 +2009,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2023,7 +2020,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2034,7 +2031,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2045,7 +2042,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Did one More Question in 450 DSA 'Next Permutation'
</commit_message>
<xml_diff>
--- a/Codes/FINAL450.xlsx
+++ b/Codes/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\Git\Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499E666-4505-425A-AD6C-167049059B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1559B294-9CC1-4E0A-A842-5F94B34386C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1887,9 +1887,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="C5" s="4" t="s">
-        <v>465</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
@@ -1899,7 +1897,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1910,7 +1908,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -2053,7 +2051,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Did some Question from 450 DSA 1) Count Inversion 2)Best time to buy and sell Stock 3)Rotate Matrix
</commit_message>
<xml_diff>
--- a/Codes/FINAL450.xlsx
+++ b/Codes/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\Git\Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1559B294-9CC1-4E0A-A842-5F94B34386C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E47FE6-28E0-4E9D-8957-5B0A3200BF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1423,6 +1423,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1854,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2062,7 +2065,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2073,7 +2076,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2383,7 +2386,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Did one Question in 450 DSA Find in 2D Matrix and added its code file
</commit_message>
<xml_diff>
--- a/Codes/FINAL450.xlsx
+++ b/Codes/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishe\Desktop\Git\Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E47FE6-28E0-4E9D-8957-5B0A3200BF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668BE742-7621-404E-99F9-A47A957C51A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1857,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2320,7 +2320,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">

</xml_diff>